<commit_message>
✨ some improvements on SCH/STH forms.
</commit_message>
<xml_diff>
--- a/SCH & STH/sch_sth_1_site.xlsx
+++ b/SCH & STH/sch_sth_1_site.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="13980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1245,11 +1245,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1458,9 +1458,7 @@
       <c r="E6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>104</v>
-      </c>
+      <c r="F6" s="18"/>
       <c r="G6" s="14"/>
       <c r="H6" s="9"/>
       <c r="I6" s="23"/>
@@ -1489,7 +1487,9 @@
       <c r="E7" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="18" t="s">
+        <v>104</v>
+      </c>
       <c r="G7" s="14"/>
       <c r="H7" s="15" t="s">
         <v>234</v>
@@ -2061,7 +2061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>

</xml_diff>